<commit_message>
BE phase 1 finished
</commit_message>
<xml_diff>
--- a/driverEvents/src/main/resources/test-data/drivers.xlsx
+++ b/driverEvents/src/main/resources/test-data/drivers.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">pb2233ac</t>
   </si>
   <si>
-    <t xml:space="preserve">emo</t>
+    <t xml:space="preserve">Emo</t>
   </si>
   <si>
     <t xml:space="preserve">emo@att.com</t>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">b4498pe</t>
   </si>
   <si>
-    <t xml:space="preserve">dido</t>
+    <t xml:space="preserve">Dido</t>
   </si>
   <si>
     <t xml:space="preserve">dido@att.com</t>
@@ -326,7 +326,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>